<commit_message>
Updating the OAuth 2.0 package
</commit_message>
<xml_diff>
--- a/RestAPI-Test-Framework/ExecutionFiles/JiraAPI/JiraAPI.xlsx
+++ b/RestAPI-Test-Framework/ExecutionFiles/JiraAPI/JiraAPI.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="71">
   <si>
     <t>ProjectName</t>
   </si>
@@ -91,15 +91,6 @@
     <t>TestClass</t>
   </si>
   <si>
-    <t>testFinancialImpactBtn_10021</t>
-  </si>
-  <si>
-    <t>testPushRiskToProgramBtn_10022</t>
-  </si>
-  <si>
-    <t>testRiskScoreForReputationalImpact_10025</t>
-  </si>
-  <si>
     <t>Project</t>
   </si>
   <si>
@@ -110,48 +101,6 @@
   </si>
   <si>
     <t>Variablevalue</t>
-  </si>
-  <si>
-    <t>Impact_Area</t>
-  </si>
-  <si>
-    <t>Delivery Impact</t>
-  </si>
-  <si>
-    <t>delivery_Impact_Score</t>
-  </si>
-  <si>
-    <t>LivelihoodScore</t>
-  </si>
-  <si>
-    <t>Cause</t>
-  </si>
-  <si>
-    <t>Service delivery</t>
-  </si>
-  <si>
-    <t>RiskId</t>
-  </si>
-  <si>
-    <t>RSK287</t>
-  </si>
-  <si>
-    <t>testRiskScoreOfDeliveryImpact_10023</t>
-  </si>
-  <si>
-    <t>testRiskScoreOfRegulatoryImpact_10024</t>
-  </si>
-  <si>
-    <t>Regulatory Impact</t>
-  </si>
-  <si>
-    <t>Privacy</t>
-  </si>
-  <si>
-    <t>Reputational Impact</t>
-  </si>
-  <si>
-    <t>Media coverage</t>
   </si>
   <si>
     <t>BaseURI</t>
@@ -715,13 +664,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -743,7 +692,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -754,7 +703,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -765,7 +714,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -779,7 +728,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -793,7 +742,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -807,7 +756,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
@@ -825,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -842,7 +791,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -854,39 +803,39 @@
         <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C2" s="3"/>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3"/>
       <c r="E3" t="str">
@@ -894,7 +843,7 @@
         <v>createIssue</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="G3" s="4">
         <v>201</v>
@@ -902,10 +851,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C4" s="3"/>
       <c r="E4" t="str">
@@ -913,18 +862,18 @@
         <v>createIssue</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C5" s="3"/>
       <c r="E5" t="str">
@@ -932,18 +881,18 @@
         <v>createIssue</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C6" s="3"/>
       <c r="E6" t="str">
@@ -951,18 +900,18 @@
         <v>createIssue</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C7" s="3"/>
       <c r="E7" t="str">
@@ -970,36 +919,36 @@
         <v>createIssue</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C8" s="3"/>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C9" s="3"/>
       <c r="E9" t="str">
@@ -1007,7 +956,7 @@
         <v>getIssue</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="G9" s="4">
         <v>200</v>
@@ -1015,35 +964,35 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C10" s="3"/>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C11" s="3"/>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="G11" s="4">
         <v>204</v>
@@ -1051,35 +1000,35 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C12" s="3"/>
       <c r="E12" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C13" s="3"/>
       <c r="E13" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="G13" s="4">
         <v>204</v>
@@ -1087,53 +1036,53 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C14" s="3"/>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C15" s="3"/>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C16" s="3"/>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="F16" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="G16" s="4">
         <v>201</v>
@@ -1141,53 +1090,53 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C17" s="3"/>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="F17" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C18" s="3"/>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="F18" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C19" s="3"/>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="F19" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="G19" s="4">
         <v>200</v>
@@ -1195,53 +1144,53 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C20" s="3"/>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="F20" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C21" s="3"/>
       <c r="E21" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="F21" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C22" s="3"/>
       <c r="E22" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="F22" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="G22" s="4">
         <v>204</v>
@@ -1249,35 +1198,35 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C23" s="3"/>
       <c r="E23" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F23" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C24" s="3"/>
       <c r="E24" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F24" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="G24" s="4">
         <v>200</v>
@@ -1285,367 +1234,108 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C25" s="3"/>
       <c r="E25" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F25" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C26" s="3"/>
       <c r="E26" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F26" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" t="s">
-        <v>51</v>
-      </c>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="3"/>
-      <c r="E27" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" t="s">
-        <v>51</v>
-      </c>
+    </row>
+    <row r="28" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="3"/>
-      <c r="E28" t="s">
-        <v>21</v>
-      </c>
-      <c r="F28" t="s">
-        <v>33</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" t="s">
-        <v>51</v>
-      </c>
+    </row>
+    <row r="29" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="3"/>
-      <c r="E29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29" t="s">
-        <v>33</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" t="s">
-        <v>51</v>
-      </c>
+    </row>
+    <row r="30" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="3"/>
-      <c r="E30" t="s">
-        <v>35</v>
-      </c>
-      <c r="F30" t="s">
-        <v>27</v>
-      </c>
-      <c r="G30" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" t="s">
-        <v>51</v>
-      </c>
+    </row>
+    <row r="31" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C31" s="3"/>
-      <c r="E31" t="str">
-        <f>(E30)</f>
-        <v>testRiskScoreOfDeliveryImpact_10023</v>
-      </c>
-      <c r="F31" t="s">
-        <v>29</v>
-      </c>
-      <c r="G31" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32" t="s">
-        <v>51</v>
-      </c>
+    </row>
+    <row r="32" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C32" s="3"/>
-      <c r="E32" t="str">
-        <f t="shared" ref="E32:E33" si="1">(E31)</f>
-        <v>testRiskScoreOfDeliveryImpact_10023</v>
-      </c>
-      <c r="F32" t="s">
-        <v>30</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B33" t="s">
-        <v>51</v>
-      </c>
+    </row>
+    <row r="33" spans="3:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C33" s="3"/>
-      <c r="E33" t="str">
-        <f t="shared" si="1"/>
-        <v>testRiskScoreOfDeliveryImpact_10023</v>
-      </c>
-      <c r="F33" t="s">
-        <v>31</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" t="s">
-        <v>51</v>
-      </c>
+    </row>
+    <row r="34" spans="3:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C34" s="3"/>
-      <c r="E34" t="s">
-        <v>36</v>
-      </c>
-      <c r="F34" t="s">
-        <v>33</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35" t="s">
-        <v>51</v>
-      </c>
+    </row>
+    <row r="35" spans="3:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C35" s="3"/>
-      <c r="E35" t="str">
-        <f>(E34)</f>
-        <v>testRiskScoreOfRegulatoryImpact_10024</v>
-      </c>
-      <c r="F35" t="s">
-        <v>27</v>
-      </c>
-      <c r="G35" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>50</v>
-      </c>
-      <c r="B36" t="s">
-        <v>51</v>
-      </c>
+    </row>
+    <row r="36" spans="3:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C36" s="3"/>
-      <c r="E36" t="str">
-        <f t="shared" ref="E36:E38" si="2">(E35)</f>
-        <v>testRiskScoreOfRegulatoryImpact_10024</v>
-      </c>
-      <c r="F36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G36" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" t="s">
-        <v>51</v>
-      </c>
+    </row>
+    <row r="37" spans="3:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C37" s="3"/>
-      <c r="E37" t="str">
-        <f t="shared" si="2"/>
-        <v>testRiskScoreOfRegulatoryImpact_10024</v>
-      </c>
-      <c r="F37" t="s">
-        <v>30</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" t="s">
-        <v>51</v>
-      </c>
+    </row>
+    <row r="38" spans="3:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C38" s="3"/>
-      <c r="E38" t="str">
-        <f t="shared" si="2"/>
-        <v>testRiskScoreOfRegulatoryImpact_10024</v>
-      </c>
-      <c r="F38" t="s">
-        <v>31</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>50</v>
-      </c>
-      <c r="B39" t="s">
-        <v>51</v>
-      </c>
+    </row>
+    <row r="39" spans="3:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C39" s="3"/>
-      <c r="E39" t="s">
-        <v>22</v>
-      </c>
-      <c r="F39" t="s">
-        <v>33</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40" t="s">
-        <v>51</v>
-      </c>
+    </row>
+    <row r="40" spans="3:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C40" s="3"/>
-      <c r="E40" t="s">
-        <v>22</v>
-      </c>
-      <c r="F40" t="s">
-        <v>27</v>
-      </c>
-      <c r="G40" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" t="s">
-        <v>51</v>
-      </c>
+    </row>
+    <row r="41" spans="3:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C41" s="3"/>
-      <c r="E41" t="s">
-        <v>22</v>
-      </c>
-      <c r="F41" t="s">
-        <v>29</v>
-      </c>
-      <c r="G41" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" t="s">
-        <v>51</v>
-      </c>
+    </row>
+    <row r="42" spans="3:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="3"/>
-      <c r="E42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F42" t="s">
-        <v>30</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>50</v>
-      </c>
-      <c r="B43" t="s">
-        <v>51</v>
-      </c>
+    </row>
+    <row r="43" spans="3:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C43" s="3"/>
-      <c r="E43" t="s">
-        <v>22</v>
-      </c>
-      <c r="F43" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C44" s="3"/>
       <c r="E44" s="2"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C45" s="3"/>
       <c r="E45" s="2"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C46" s="3"/>
       <c r="E46" s="2"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C47" s="3"/>
       <c r="E47" s="2"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C48" s="3"/>
       <c r="E48" s="2"/>
     </row>

</xml_diff>